<commit_message>
Rename newlink.Stream -> ServerStream; fix many comments that mention Stream/ServerStream/ClientStream/stream
</commit_message>
<xml_diff>
--- a/docs/website/protocol.xlsx
+++ b/docs/website/protocol.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="11880" windowHeight="7335"/>
@@ -307,9 +307,6 @@
     </r>
   </si>
   <si>
-    <t>Sent to indicate that a Stream has been successfully created. This is the first frame sent over *every* sucessfully-authenticated transport with `requestNewStream`, so it may be sent over more than one in transport. This allows the client to know that it can now send smaller HelloFrames without `requestNewStream` and `credentialsData`.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -423,6 +420,9 @@
   </si>
   <si>
     <t>CommentFrame is used for HTTP anti-script-inclusion preamble, padding, and heartbeats.  Padding is only needed to work around browser problems with content sniffing (in IE, Safari, Chrome, maybe Opera?), and maybe annoying proxies.</t>
+  </si>
+  <si>
+    <t>Sent to indicate that a ServerStream has been successfully created. This is the first frame sent over *every* sucessfully-authenticated transport with `requestNewStream`, so it may be sent over more than one in transport. This allows the client to know that it can now send smaller HelloFrames without `requestNewStream` and `credentialsData`.</t>
   </si>
 </sst>
 </file>
@@ -920,7 +920,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -937,7 +937,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -960,7 +960,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
@@ -1000,27 +1000,27 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1060,7 +1060,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
@@ -1080,7 +1080,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1120,7 +1120,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
@@ -1140,7 +1140,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
@@ -1160,12 +1160,12 @@
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>2</v>
@@ -1220,7 +1220,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
@@ -1245,7 +1245,7 @@
     </row>
     <row r="19" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
       <c r="F19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1260,7 +1260,7 @@
     </row>
     <row r="23" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="F23" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1290,8 +1290,9 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <webPublishItems count="1">
-    <webPublishItem id="10526" divId="protocol_10526" sourceType="sheet" destinationFile="L:\home\at\Projects\Minerva\docs\protocol.htm" autoRepublish="1"/>
+  <webPublishItems count="2">
+    <webPublishItem id="10526" divId="protocol_10526" sourceType="sheet" destinationFile="C:\Users\root\Documents\Projects\Minerva\docs\protocol.htm" autoRepublish="1"/>
+    <webPublishItem id="25772" divId="protocol_25772" sourceType="sheet" destinationFile="C:\Users\root\Documents\Projects\Minerva\docs\protocol.htm" autoRepublish="1"/>
   </webPublishItems>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Remove all mentions of 'box' from Minerva.  Boxes were replaced with restricted strings a while ago, due to the complexity of doing JSON encoding/decoding for the user.
</commit_message>
<xml_diff>
--- a/docs/website/protocol.xlsx
+++ b/docs/website/protocol.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Protocol" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -49,9 +47,6 @@
     <t>"The next string I write to the transport will have this seqNum"</t>
   </si>
   <si>
-    <t>This error is a response to client sending a SackFrame that SACKed strings that server never sent. Only the server sends acked_unsent_boxes. If the client thinks server sent a bad SACK, it should send ResetFrame.</t>
-  </si>
-  <si>
     <t>This error is a response to client sending corrupt frame octets or an overlong frame. Only server sends frame_corruption. If client received corrupt frames, it should make a new transport.</t>
   </si>
   <si>
@@ -332,9 +327,6 @@
     <t>This error is a response to client sending any unknown frame, or frame with invalid arguments. Only server sends invalid_frame_type_or_arguments. Only server sends invalid_frame_type_or_arguments. If client gets an unknown frame type or bad arguments, it should make a new transport.</t>
   </si>
   <si>
-    <t>Both peers send strings (previously "boxes") - every other frame supports this basic function. `string` is restricted to the base "restricted string" codepoints.</t>
-  </si>
-  <si>
     <t>Either peer can reset if they've given up on this stream. `reasonString` is restricted to the base "restricted string" codepoints.</t>
   </si>
   <si>
@@ -393,36 +385,42 @@
     <t>This error is a possible response to HelloFrame. It means transport authentication failed, or streamId does not exist.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>CommentFrame</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(comment)</t>
+    </r>
+  </si>
+  <si>
+    <t>CommentFrame is used for HTTP anti-script-inclusion preamble, padding, and heartbeats.  Padding is only needed to work around browser problems with content sniffing (in IE, Safari, Chrome, maybe Opera?), and maybe annoying proxies.</t>
+  </si>
+  <si>
+    <t>Sent to indicate that a ServerStream has been successfully created. This is the first frame sent over *every* sucessfully-authenticated transport with `requestNewStream`, so it may be sent over more than one in transport. This allows the client to know that it can now send smaller HelloFrames without `requestNewStream` and `credentialsData`.</t>
+  </si>
+  <si>
+    <t>Both peers send strings - every other frame supports this basic function. `string` is restricted to the base "restricted string" codepoints.</t>
+  </si>
+  <si>
+    <t>This error is a response to client sending a SackFrame that SACKed strings that server never sent. Only the server sends acked_unsent_strings. If the client thinks server sent a bad SACK, it should send ResetFrame.</t>
+  </si>
+  <si>
     <t>HelloFrame arguments are documented in frames.py and frames.js
-Presence of succeedsTransport option means "give me boxes, server". If succeedsTransport != null, temporarily assume that all boxes written to #&lt;succeedsTransport&gt; were SACKed.
+Presence of succeedsTransport option means "give me strings, server". If succeedsTransport != null, temporarily assume that all strings written to #&lt;succeedsTransport&gt; were SACKed.
 Idea: perhaps ackMode: 0 - require Minerva-level SACKs, 1 - use my TCP acks, 2 - assume everything written is received</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>CommentFrame</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>(comment)</t>
-    </r>
-  </si>
-  <si>
-    <t>CommentFrame is used for HTTP anti-script-inclusion preamble, padding, and heartbeats.  Padding is only needed to work around browser problems with content sniffing (in IE, Safari, Chrome, maybe Opera?), and maybe annoying proxies.</t>
-  </si>
-  <si>
-    <t>Sent to indicate that a ServerStream has been successfully created. This is the first frame sent over *every* sucessfully-authenticated transport with `requestNewStream`, so it may be sent over more than one in transport. This allows the client to know that it can now send smaller HelloFrames without `requestNewStream` and `credentialsData`.</t>
   </si>
 </sst>
 </file>
@@ -919,9 +917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -930,14 +926,14 @@
     <col min="3" max="3" width="4.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="5.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="104.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="92.5703125" style="2" customWidth="1"/>
     <col min="7" max="9" width="94" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -960,12 +956,12 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>1</v>
@@ -980,12 +976,12 @@
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>2</v>
@@ -1000,12 +996,12 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>2</v>
@@ -1020,12 +1016,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>1</v>
@@ -1045,7 +1041,7 @@
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>1</v>
@@ -1060,12 +1056,12 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>1</v>
@@ -1080,12 +1076,12 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>1</v>
@@ -1100,12 +1096,12 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>2</v>
@@ -1120,12 +1116,12 @@
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>2</v>
@@ -1140,12 +1136,12 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>2</v>
@@ -1160,12 +1156,12 @@
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>2</v>
@@ -1180,12 +1176,12 @@
         <v>1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>2</v>
@@ -1200,12 +1196,12 @@
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>2</v>
@@ -1220,12 +1216,12 @@
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>2</v>
@@ -1240,17 +1236,17 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="76.5" x14ac:dyDescent="0.25">
       <c r="F19" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1260,7 +1256,7 @@
     </row>
     <row r="23" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
       <c r="F23" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1295,28 +1291,4 @@
     <webPublishItem id="25772" divId="protocol_25772" sourceType="sheet" destinationFile="C:\Users\root\Documents\Projects\Minerva\docs\protocol.htm" autoRepublish="1"/>
   </webPublishItems>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>